<commit_message>
drop aggregate type from freq figures
</commit_message>
<xml_diff>
--- a/info_sheets/Datasets.xlsx
+++ b/info_sheets/Datasets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gamal Elkoumy\PhD\OneDrive - Tartu Ülikool\Differential Privacy\source code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gamal Elkoumy\PhD\OneDrive - Tartu Ülikool\Differential Privacy\source code\info_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECB1207-7132-484F-8ABB-3C754A763F3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC0D9F0-B3AC-49DE-8301-0C312E51E958}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2D5D8AB6-B5FA-4CBE-B210-E3C0BAD95574}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2D5D8AB6-B5FA-4CBE-B210-E3C0BAD95574}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,12 +100,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -135,14 +141,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -462,18 +472,18 @@
   <dimension ref="A2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +503,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -513,67 +523,67 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>115</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>16</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>15214</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="5">
         <v>1050</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="4">
         <v>846</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>3830</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>376</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>33373</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>645</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="4">
         <v>644</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
         <v>4802</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>410</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>44354</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="4">
         <v>832</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="4">
         <v>828</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -593,7 +603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -613,7 +623,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -633,7 +643,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>